<commit_message>
trival work in the past month
</commit_message>
<xml_diff>
--- a/文档/火车票管理系统 开发进度.xlsx
+++ b/文档/火车票管理系统 开发进度.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\TicketSystem\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDE7EB9-AF2B-4523-BD6F-7D3E3BAC7F87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24A2B8D-B435-4C86-A050-47717B9DA4DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
   <si>
     <t>火车票管理系统 开发进度</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,10 +68,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>login.php(包括session，cookie)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>logout.php(包括session，cookie销毁)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -120,10 +116,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>trainadd.html/js（添加车次）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>trainadd.php（添加车次）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -236,19 +228,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>userman.html/js（用户信息查询修改，包含了ticket_query_order和refund_ticket）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.5  5.21</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>listener.cpp(exe) 已为clion和cmakelist提供支持</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>5.21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.5  6.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端独立版本 main.cpp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login.js(新增用js控制html表单，前端过滤空格等异常字符)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.5  5.21  6.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userman.html/js（用户信息查询修改，包含了ticket_query_order和refund_ticket）（6.10新增滑动效果）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main.cpp为解决utf8问题转为linux平台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.12  6.11  6.16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login.php(包括session，cookie)（6.12为移动端提供支持）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.6  6.10  6.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>trainadd.html/js（添加车次） （6.11新增图形化添加页面，js完全控制表单）（6.16修复清空的bug，确保动态站点不会出现问题）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -776,15 +812,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="78.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="113.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.75" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
@@ -811,7 +847,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -819,16 +855,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -840,7 +876,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -848,10 +884,10 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E5" s="5"/>
     </row>
@@ -859,10 +895,10 @@
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E6" s="5"/>
     </row>
@@ -870,34 +906,34 @@
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="5"/>
-      <c r="B8" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C9" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E9" s="5"/>
     </row>
@@ -905,10 +941,10 @@
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E10" s="5"/>
     </row>
@@ -916,10 +952,10 @@
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="E11" s="5"/>
     </row>
@@ -927,34 +963,34 @@
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="5"/>
-      <c r="B13" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="B13" s="5"/>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -962,10 +998,10 @@
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="5"/>
     </row>
@@ -973,10 +1009,10 @@
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="5"/>
     </row>
@@ -984,10 +1020,10 @@
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E17" s="5"/>
     </row>
@@ -995,10 +1031,10 @@
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="E18" s="5"/>
     </row>
@@ -1006,10 +1042,10 @@
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E19" s="5"/>
     </row>
@@ -1017,34 +1053,34 @@
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="5"/>
-      <c r="B21" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="B21" s="5"/>
       <c r="C21" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E22" s="5"/>
     </row>
@@ -1052,10 +1088,10 @@
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E23" s="5"/>
     </row>
@@ -1063,10 +1099,10 @@
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E24" s="5"/>
     </row>
@@ -1074,10 +1110,10 @@
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E25" s="5"/>
     </row>
@@ -1085,10 +1121,10 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E26" s="5"/>
     </row>
@@ -1096,10 +1132,10 @@
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E27" s="5"/>
     </row>
@@ -1107,10 +1143,10 @@
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -1118,10 +1154,10 @@
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -1129,16 +1165,22 @@
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="5"/>
-      <c r="D31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="5"/>
@@ -1151,13 +1193,13 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="5"/>
       <c r="B34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="D34" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
@@ -1175,31 +1217,45 @@
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="D39" s="4"/>
-    </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="D40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D41" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A38:B40"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B13:B20"/>
     <mergeCell ref="A3:A34"/>
-    <mergeCell ref="B21:B30"/>
     <mergeCell ref="E3:E30"/>
+    <mergeCell ref="B22:B31"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B4:B8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
stable frontend version 1.0
</commit_message>
<xml_diff>
--- a/文档/火车票管理系统 开发进度.xlsx
+++ b/文档/火车票管理系统 开发进度.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\TicketSystem\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24A2B8D-B435-4C86-A050-47717B9DA4DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD62E2D-6A91-403E-A377-404400416E1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="3615" windowWidth="19710" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>火车票管理系统 开发进度</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -285,6 +285,26 @@
   </si>
   <si>
     <t>trainadd.html/js（添加车次） （6.11新增图形化添加页面，js完全控制表单）（6.16修复清空的bug，确保动态站点不会出现问题）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>todo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.php socket扩容！！！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. tranfer 重写</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. train inquire 阶梯表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 购买车票 今日以前</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -810,13 +830,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.75" style="1" customWidth="1"/>
@@ -1245,6 +1265,31 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D41" s="4"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C44" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C45" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C46" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C47" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C48" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>